<commit_message>
UlTiM_bus layout, gerber complete. Bus accessory for ULTiM8x8
</commit_message>
<xml_diff>
--- a/kicad/PCB Technology Requirement Format V1 for ultim8x8.xlsx
+++ b/kicad/PCB Technology Requirement Format V1 for ultim8x8.xlsx
@@ -5,19 +5,31 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>                         深圳矽递科技有限公司
                           </t>
     </r>
@@ -39,10 +51,18 @@
     <t>PCB Name &amp; Version</t>
   </si>
   <si>
-    <t>TinyTim_rev3</t>
-  </si>
-  <si>
-    <r>
+    <t>ULTiM8x8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>PCB Material
 PCB</t>
     </r>
@@ -53,12 +73,20 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>板材：</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>  
     (Rigid)FR</t>
     </r>
@@ -66,8 +94,9 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>－</t>
     </r>
@@ -85,6 +114,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>PCB Size
 PCB</t>
     </r>
@@ -95,6 +132,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>大小：</t>
     </r>
@@ -103,10 +141,18 @@
     <t> inch</t>
   </si>
   <si>
-    <t>( 4.80 ) × (4.80 )</t>
-  </si>
-  <si>
-    <r>
+    <t>( 2.40 ) × (2.40 )</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>PCB  Layer
 PCB</t>
     </r>
@@ -117,12 +163,21 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>层数：</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Thickness
 PCB</t>
     </r>
@@ -133,15 +188,24 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>厚度：</t>
     </r>
   </si>
   <si>
-    <t>    1mm </t>
-  </si>
-  <si>
-    <r>
+    <t>1.6mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Copper Weight
 </t>
     </r>
@@ -152,15 +216,24 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>铜厚：</t>
     </r>
   </si>
   <si>
-    <t> 2oz</t>
-  </si>
-  <si>
-    <r>
+    <t>1oz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>PCB Colour
 </t>
     </r>
@@ -171,15 +244,43 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>阻焊颜色：</t>
     </r>
   </si>
   <si>
-    <t>other:( CLEAR )</t>
-  </si>
-  <si>
-    <r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>White</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>白色</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Silkscreen
 </t>
     </r>
@@ -190,12 +291,20 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>字符颜色：</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Black
 </t>
     </r>
@@ -205,6 +314,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>黑色</t>
     </r>
@@ -214,6 +324,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Pads Finished
 </t>
     </r>
@@ -224,12 +342,20 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>焊盘喷镀：</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t> (Hasl-lead free)   
 </t>
     </r>
@@ -239,12 +365,21 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>无铅喷锡</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Via solder mask
 </t>
     </r>
@@ -255,12 +390,20 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>阻焊覆盖：</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>solder mask  opening 
 </t>
     </r>
@@ -270,12 +413,21 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>过孔开窗</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Minimum trace/space
 (mm)
 </t>
@@ -287,12 +439,24 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>最小线宽</t>
     </r>
   </si>
   <si>
-    <r>
+    <t>0.254mm/0.254mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Minimum hole size
 (mm)
 </t>
@@ -304,12 +468,24 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>最小孔径</t>
     </r>
   </si>
   <si>
-    <r>
+    <t>0.635mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Special requirements
 </t>
     </r>
@@ -320,22 +496,19 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>特殊工艺：</t>
     </r>
   </si>
   <si>
-    <t> Yes</t>
+    <t>No</t>
   </si>
   <si>
     <t>(Put requirements here)</t>
   </si>
   <si>
     <t>Comment:</t>
-  </si>
-  <si>
-    <t>NOTE : SILK SCREEN is ONLY on BOTTOM Layer.
-FRONT Layer NO SILKSCREEN</t>
   </si>
 </sst>
 </file>
@@ -372,15 +545,16 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Droid Sans Fallback"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -412,6 +586,7 @@
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -564,11 +739,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,15 +763,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -608,43 +783,43 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,7 +827,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,7 +835,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,15 +916,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>65160</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>697680</xdr:colOff>
+      <xdr:colOff>724320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>476280</xdr:rowOff>
+      <xdr:rowOff>466920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -762,8 +937,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="65160" y="38520"/>
-          <a:ext cx="632520" cy="437760"/>
+          <a:off x="92160" y="29520"/>
+          <a:ext cx="632160" cy="437400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -785,19 +960,19 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2550607287449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.3765182186235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3724696356275"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2226720647773"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.9109311740891"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6234817813765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.5951417004049"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.080971659919"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.68421052631579"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -910,10 +1085,10 @@
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="12"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -925,7 +1100,9 @@
         <v>14</v>
       </c>
       <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="19"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -936,9 +1113,7 @@
       <c r="A11" s="6"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -980,31 +1155,33 @@
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="C15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="21"/>
+        <v>25</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
     </row>

</xml_diff>